<commit_message>
Include x, y coordinates into Cell object to increase efficiency
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Students!$F$6:$I$16</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -736,6 +739,7 @@
       <c r="I15" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="F6:I16"/>
   <mergeCells count="4">
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="I10:I11"/>

</xml_diff>